<commit_message>
Fixed Cymax Suite Issue
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/FCFile.xlsx
+++ b/binaries/FCfiles/FCFile.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="103">
   <si>
     <t>shipmentType</t>
   </si>
@@ -339,6 +339,18 @@
   </si>
   <si>
     <t>51471598</t>
+  </si>
+  <si>
+    <t>51472140</t>
+  </si>
+  <si>
+    <t>51472141</t>
+  </si>
+  <si>
+    <t>51472467</t>
+  </si>
+  <si>
+    <t>51472468</t>
   </si>
 </sst>
 </file>
@@ -556,7 +568,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="169">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -610,6 +622,20 @@
     <xf applyBorder="1" applyFill="1" borderId="13" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="13" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="13" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
@@ -1121,8 +1147,8 @@
       <c r="O2" s="6">
         <v>1</v>
       </c>
-      <c r="P2" s="151" t="s">
-        <v>95</v>
+      <c r="P2" s="165" t="s">
+        <v>101</v>
       </c>
     </row>
     <row customFormat="1" r="3" s="6" spans="1:17">
@@ -1165,8 +1191,8 @@
       <c r="O3" s="6">
         <v>1</v>
       </c>
-      <c r="P3" s="152" t="s">
-        <v>96</v>
+      <c r="P3" s="166" t="s">
+        <v>102</v>
       </c>
     </row>
     <row customFormat="1" r="4" s="6" spans="1:17">
@@ -1215,8 +1241,8 @@
       <c r="O4" s="6">
         <v>2</v>
       </c>
-      <c r="P4" s="153" t="s">
-        <v>97</v>
+      <c r="P4" s="167" t="s">
+        <v>83</v>
       </c>
       <c r="Q4" s="15"/>
     </row>
@@ -1266,8 +1292,8 @@
       <c r="O5" s="6">
         <v>2</v>
       </c>
-      <c r="P5" s="154" t="s">
-        <v>98</v>
+      <c r="P5" s="168" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed all FC Ph1 and Ph2
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/FCFile.xlsx
+++ b/binaries/FCfiles/FCFile.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="113">
   <si>
     <t>shipmentType</t>
   </si>
@@ -351,6 +351,36 @@
   </si>
   <si>
     <t>51472468</t>
+  </si>
+  <si>
+    <t>51475745</t>
+  </si>
+  <si>
+    <t>51475746</t>
+  </si>
+  <si>
+    <t>51475747</t>
+  </si>
+  <si>
+    <t>51475748</t>
+  </si>
+  <si>
+    <t>51475757</t>
+  </si>
+  <si>
+    <t>51475758</t>
+  </si>
+  <si>
+    <t>51475869</t>
+  </si>
+  <si>
+    <t>51475870</t>
+  </si>
+  <si>
+    <t>51475871</t>
+  </si>
+  <si>
+    <t>51475872</t>
   </si>
 </sst>
 </file>
@@ -568,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="198">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -622,6 +652,35 @@
     <xf applyBorder="1" applyFill="1" borderId="13" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="13" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="13" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
@@ -1147,8 +1206,8 @@
       <c r="O2" s="6">
         <v>1</v>
       </c>
-      <c r="P2" s="165" t="s">
-        <v>101</v>
+      <c r="P2" s="191" t="s">
+        <v>109</v>
       </c>
     </row>
     <row customFormat="1" r="3" s="6" spans="1:17">
@@ -1191,8 +1250,8 @@
       <c r="O3" s="6">
         <v>1</v>
       </c>
-      <c r="P3" s="166" t="s">
-        <v>102</v>
+      <c r="P3" s="193" t="s">
+        <v>110</v>
       </c>
     </row>
     <row customFormat="1" r="4" s="6" spans="1:17">
@@ -1241,8 +1300,8 @@
       <c r="O4" s="6">
         <v>2</v>
       </c>
-      <c r="P4" s="167" t="s">
-        <v>83</v>
+      <c r="P4" s="195" t="s">
+        <v>111</v>
       </c>
       <c r="Q4" s="15"/>
     </row>
@@ -1292,8 +1351,8 @@
       <c r="O5" s="6">
         <v>2</v>
       </c>
-      <c r="P5" s="168" t="s">
-        <v>83</v>
+      <c r="P5" s="197" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merging of all the FC suites
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/FCFile.xlsx
+++ b/binaries/FCfiles/FCFile.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView tabRatio="449" windowHeight="11760" windowWidth="20730" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" tabRatio="449" windowHeight="11760" windowWidth="20730" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Input" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet1" r:id="rId2" sheetId="3"/>
-    <sheet name="Legend" r:id="rId3" sheetId="2"/>
-    <sheet name="Marrkups" r:id="rId4" sheetId="4"/>
+    <sheet name="CreateAccount" r:id="rId1" sheetId="5"/>
+    <sheet name="ShipmentInformation" r:id="rId2" sheetId="6"/>
+    <sheet name="Input" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet1" r:id="rId4" sheetId="3"/>
+    <sheet name="Legend" r:id="rId5" sheetId="2"/>
+    <sheet name="Marrkups" r:id="rId6" sheetId="4"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="157">
   <si>
     <t>shipmentType</t>
   </si>
@@ -299,88 +301,220 @@
     <t>Bagged or Unboxed Product</t>
   </si>
   <si>
-    <t>51470874</t>
-  </si>
-  <si>
-    <t>51470875</t>
-  </si>
-  <si>
-    <t>51470876</t>
-  </si>
-  <si>
-    <t>51470877</t>
-  </si>
-  <si>
-    <t>51470878</t>
-  </si>
-  <si>
-    <t>51471036</t>
-  </si>
-  <si>
-    <t>51471550</t>
-  </si>
-  <si>
-    <t>51471551</t>
-  </si>
-  <si>
-    <t>51471552</t>
-  </si>
-  <si>
-    <t>51471553</t>
-  </si>
-  <si>
-    <t>51471595</t>
-  </si>
-  <si>
-    <t>51471596</t>
-  </si>
-  <si>
-    <t>51471597</t>
-  </si>
-  <si>
-    <t>51471598</t>
-  </si>
-  <si>
-    <t>51472140</t>
-  </si>
-  <si>
-    <t>51472141</t>
-  </si>
-  <si>
-    <t>51472467</t>
-  </si>
-  <si>
-    <t>51472468</t>
-  </si>
-  <si>
-    <t>51475745</t>
-  </si>
-  <si>
-    <t>51475746</t>
-  </si>
-  <si>
-    <t>51475747</t>
-  </si>
-  <si>
-    <t>51475748</t>
-  </si>
-  <si>
-    <t>51475757</t>
-  </si>
-  <si>
-    <t>51475758</t>
-  </si>
-  <si>
-    <t>51475869</t>
-  </si>
-  <si>
-    <t>51475870</t>
-  </si>
-  <si>
-    <t>51475871</t>
-  </si>
-  <si>
-    <t>51475872</t>
+    <t>packageType2</t>
+  </si>
+  <si>
+    <t>SearchaddedProduct</t>
+  </si>
+  <si>
+    <t>Addproductonstep3</t>
+  </si>
+  <si>
+    <t>Non-Palletized</t>
+  </si>
+  <si>
+    <t>AccountType</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Automation</t>
+  </si>
+  <si>
+    <t>Test Automation</t>
+  </si>
+  <si>
+    <t>9154169799</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>Automation123!</t>
+  </si>
+  <si>
+    <t>SpecialHandlingInstructions</t>
+  </si>
+  <si>
+    <t>AddressLine1</t>
+  </si>
+  <si>
+    <t>AddressLine2</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>ZipCode</t>
+  </si>
+  <si>
+    <t>Test Description</t>
+  </si>
+  <si>
+    <t>Test AddressLine1</t>
+  </si>
+  <si>
+    <t>Test AddressLine2</t>
+  </si>
+  <si>
+    <t>Test State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Country </t>
+  </si>
+  <si>
+    <t>Test City</t>
+  </si>
+  <si>
+    <t>TestEmail@gmail.com</t>
+  </si>
+  <si>
+    <t>Test SpecialHandlingInstructions</t>
+  </si>
+  <si>
+    <t>PickUpAddressLine1</t>
+  </si>
+  <si>
+    <t>PickUpFirstName</t>
+  </si>
+  <si>
+    <t>PickUpLastName</t>
+  </si>
+  <si>
+    <t>DropOffAddressLine1</t>
+  </si>
+  <si>
+    <t>DropOffFirstname</t>
+  </si>
+  <si>
+    <t>DropOffLastName</t>
+  </si>
+  <si>
+    <t>DropOffPhone1</t>
+  </si>
+  <si>
+    <t>Test PickUpAddressLine1</t>
+  </si>
+  <si>
+    <t>Test PickUpFirstName</t>
+  </si>
+  <si>
+    <t>Test PickupLastName</t>
+  </si>
+  <si>
+    <t>PickUpPhone1</t>
+  </si>
+  <si>
+    <t>Test DropOffAddressLine1</t>
+  </si>
+  <si>
+    <t>Test DropOffFirstName</t>
+  </si>
+  <si>
+    <t>Test DropOffLastName</t>
+  </si>
+  <si>
+    <t>9154159698</t>
+  </si>
+  <si>
+    <t>1234567890</t>
+  </si>
+  <si>
+    <t>TestOrder1</t>
+  </si>
+  <si>
+    <t>TestOrder2</t>
+  </si>
+  <si>
+    <t>TestOrder3</t>
+  </si>
+  <si>
+    <t>TestOrder4</t>
+  </si>
+  <si>
+    <t>TestOrder5</t>
+  </si>
+  <si>
+    <t>TestOrder6</t>
+  </si>
+  <si>
+    <t>TestOrder7</t>
+  </si>
+  <si>
+    <t>TestOrder8</t>
+  </si>
+  <si>
+    <t>TestOrder9</t>
+  </si>
+  <si>
+    <t>TestOrder10</t>
+  </si>
+  <si>
+    <t>TestOrder11</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>51480497</t>
+  </si>
+  <si>
+    <t>51480498</t>
+  </si>
+  <si>
+    <t>51480504</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>51482047</t>
+  </si>
+  <si>
+    <t>51482052</t>
+  </si>
+  <si>
+    <t>51482055</t>
+  </si>
+  <si>
+    <t>51482058</t>
+  </si>
+  <si>
+    <t>51482061</t>
   </si>
 </sst>
 </file>
@@ -388,13 +522,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -432,7 +573,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -588,6 +729,28 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <top style="thin"/>
     </border>
     <border>
@@ -595,10 +758,14 @@
       <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="90">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -648,161 +815,54 @@
     <xf applyBorder="1" applyFill="1" borderId="1" fillId="5" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="13" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="13" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="13" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="13" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="1" borderId="13" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyFill="1" borderId="14" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="14" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="14" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="14" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="14" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="14" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="14" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="15" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1081,10 +1141,235 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="W5" sqref="W5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="5.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="46" width="14.140625" collapsed="true"/>
+    <col min="9" max="9" style="46" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="46" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="46" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" t="s">
+        <v>93</v>
+      </c>
+      <c r="J1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K1" t="s">
+        <v>97</v>
+      </c>
+      <c r="L1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M1" t="s">
+        <v>121</v>
+      </c>
+      <c r="N1" t="s">
+        <v>122</v>
+      </c>
+      <c r="O1" t="s">
+        <v>130</v>
+      </c>
+      <c r="P1" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>124</v>
+      </c>
+      <c r="R1" t="s">
+        <v>125</v>
+      </c>
+      <c r="S1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="J2" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="K2" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="L2" t="s">
+        <v>127</v>
+      </c>
+      <c r="M2" t="s">
+        <v>128</v>
+      </c>
+      <c r="N2" t="s">
+        <v>129</v>
+      </c>
+      <c r="O2" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="P2" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>132</v>
+      </c>
+      <c r="R2" t="s">
+        <v>133</v>
+      </c>
+      <c r="S2" s="46" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="I2"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1096,18 +1381,19 @@
     <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="11.28515625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="10.7109375" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="12.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="4" width="33.42578125" collapsed="true"/>
-    <col min="9" max="11" style="4" width="9.140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="4" width="11.85546875" collapsed="true"/>
-    <col min="13" max="13" style="4" width="9.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="4" width="14.140625" collapsed="true"/>
-    <col min="15" max="15" style="4" width="9.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="4" width="9.95703125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="4" width="9.28515625" collapsed="true"/>
-    <col min="18" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" style="4" width="33.42578125" collapsed="true"/>
+    <col min="10" max="12" style="4" width="9.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="4" width="11.85546875" collapsed="true"/>
+    <col min="14" max="14" style="4" width="9.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="4" width="14.140625" collapsed="true"/>
+    <col min="16" max="16" style="4" width="9.140625" collapsed="true"/>
+    <col min="17" max="17" style="4" width="9.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="4" width="9.95703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="4" width="9.28515625" collapsed="true"/>
+    <col min="20" max="16384" style="4" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="6" spans="1:17">
+    <row customFormat="1" r="1" s="6" spans="1:19">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1117,13 +1403,13 @@
       <c r="C1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="6" t="s">
@@ -1133,34 +1419,40 @@
         <v>9</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="R1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="15.75" r="2" s="6" spans="1:17">
+    <row customFormat="1" customHeight="1" ht="15.75" r="2" s="6" spans="1:19">
       <c r="A2" s="6" t="s">
         <v>33</v>
       </c>
@@ -1168,49 +1460,31 @@
         <v>38</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="5" t="s">
         <v>63</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>35</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="6">
-        <v>40</v>
-      </c>
-      <c r="J2" s="6">
-        <v>65</v>
-      </c>
-      <c r="K2" s="6">
-        <v>40</v>
-      </c>
-      <c r="L2" s="6">
-        <v>40</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="N2" s="6">
-        <v>100</v>
-      </c>
-      <c r="O2" s="6">
+        <v>86</v>
+      </c>
+      <c r="Q2" s="59">
         <v>1</v>
       </c>
-      <c r="P2" s="191" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row customFormat="1" r="3" s="6" spans="1:17">
+      <c r="R2" s="89" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row customFormat="1" r="3" s="6" spans="1:19">
       <c r="A3" s="6" t="s">
         <v>33</v>
       </c>
@@ -1218,15 +1492,15 @@
         <v>38</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="5" t="s">
         <v>63</v>
       </c>
       <c r="G3" s="6" t="s">
@@ -1235,124 +1509,474 @@
       <c r="H3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J3" s="6">
         <v>40</v>
       </c>
-      <c r="L3" s="6">
+      <c r="M3" s="6">
         <v>40</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="N3" s="6">
-        <v>100</v>
-      </c>
-      <c r="O3" s="6">
+      <c r="O3" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="P3" s="6">
         <v>1</v>
       </c>
-      <c r="P3" s="193" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row customFormat="1" r="4" s="6" spans="1:17">
+      <c r="Q3" s="59">
+        <v>1</v>
+      </c>
+      <c r="R3" s="80" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row customFormat="1" customHeight="1" ht="15.75" r="4" s="6" spans="1:19">
       <c r="A4" s="6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="5" t="s">
         <v>63</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>35</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" s="6">
+        <v>88</v>
+      </c>
+      <c r="J4" s="6">
         <v>40</v>
       </c>
-      <c r="J4" s="6">
-        <v>50</v>
-      </c>
       <c r="K4" s="6">
-        <v>10</v>
-      </c>
-      <c r="L4" s="8">
-        <v>12</v>
-      </c>
-      <c r="M4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" s="6">
+        <v>40</v>
+      </c>
+      <c r="M4" s="6">
+        <v>40</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="N4" s="6">
-        <v>100</v>
-      </c>
-      <c r="O4" s="6">
-        <v>2</v>
-      </c>
-      <c r="P4" s="195" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q4" s="15"/>
-    </row>
-    <row customFormat="1" r="5" s="6" spans="1:17">
+      <c r="O4" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="P4" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="59">
+        <v>1</v>
+      </c>
+      <c r="R4" s="83" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row customFormat="1" r="5" s="6" spans="1:19">
       <c r="A5" s="6" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="5" t="s">
         <v>63</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>35</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="I5" s="6">
+        <v>88</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>40</v>
       </c>
       <c r="J5" s="6">
         <v>40</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="6">
+        <v>65</v>
+      </c>
+      <c r="L5" s="6">
         <v>40</v>
       </c>
-      <c r="L5" s="8">
+      <c r="M5" s="6">
+        <v>40</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="P5" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="59">
+        <v>1</v>
+      </c>
+      <c r="R5" s="86" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row customFormat="1" r="6" s="6" spans="1:19">
+      <c r="A6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="6">
+        <v>40</v>
+      </c>
+      <c r="K6" s="6">
+        <v>50</v>
+      </c>
+      <c r="L6" s="6">
+        <v>10</v>
+      </c>
+      <c r="M6" s="8">
         <v>12</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="N6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="N5" s="6">
-        <v>100</v>
-      </c>
-      <c r="O5" s="6">
+      <c r="O6" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="P6" s="6">
         <v>2</v>
       </c>
-      <c r="P5" s="197" t="s">
-        <v>112</v>
+      <c r="Q6" s="59">
+        <v>1</v>
+      </c>
+      <c r="R6" s="88" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row customFormat="1" r="7" s="6" spans="1:19">
+      <c r="A7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="Q7" s="59">
+        <v>1</v>
+      </c>
+      <c r="R7" s="49" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row customFormat="1" r="8" s="6" spans="1:19">
+      <c r="A8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="6">
+        <v>40</v>
+      </c>
+      <c r="K8" s="6">
+        <v>65</v>
+      </c>
+      <c r="L8" s="6">
+        <v>40</v>
+      </c>
+      <c r="M8" s="6">
+        <v>40</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="P8" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="59">
+        <v>1</v>
+      </c>
+      <c r="R8" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="S8" s="45"/>
+    </row>
+    <row customFormat="1" r="9" s="6" spans="1:19">
+      <c r="A9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="6">
+        <v>40</v>
+      </c>
+      <c r="K9" s="6">
+        <v>40</v>
+      </c>
+      <c r="L9" s="6">
+        <v>40</v>
+      </c>
+      <c r="M9" s="6">
+        <v>40</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="P9" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="59">
+        <v>1</v>
+      </c>
+      <c r="R9" s="51" t="s">
+        <v>149</v>
+      </c>
+      <c r="S9" s="15"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6">
+        <v>40</v>
+      </c>
+      <c r="K10" s="6">
+        <v>40</v>
+      </c>
+      <c r="L10" s="8">
+        <v>40</v>
+      </c>
+      <c r="M10" s="8">
+        <v>12</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="P10" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="59">
+        <v>1</v>
+      </c>
+      <c r="R10" s="52" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row customFormat="1" r="11" s="6" spans="1:19">
+      <c r="A11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" s="6">
+        <v>40</v>
+      </c>
+      <c r="K11" s="6">
+        <v>25</v>
+      </c>
+      <c r="L11" s="6">
+        <v>20</v>
+      </c>
+      <c r="M11" s="8">
+        <v>12</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="P11" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="59">
+        <v>1</v>
+      </c>
+      <c r="R11" s="53" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row customFormat="1" r="12" s="6" spans="1:19">
+      <c r="A12" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="Q12" s="59">
+        <v>1</v>
+      </c>
+      <c r="R12" s="54" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1361,12 +1985,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1617,7 +2241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -1798,12 +2422,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:O14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Merging of multiple FC suites into one
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/FCFile.xlsx
+++ b/binaries/FCfiles/FCFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="184">
   <si>
     <t>shipmentType</t>
   </si>
@@ -515,6 +515,87 @@
   </si>
   <si>
     <t>51482061</t>
+  </si>
+  <si>
+    <t>51482105</t>
+  </si>
+  <si>
+    <t>51482107</t>
+  </si>
+  <si>
+    <t>51482117</t>
+  </si>
+  <si>
+    <t>51482120</t>
+  </si>
+  <si>
+    <t>51482123</t>
+  </si>
+  <si>
+    <t>51482126</t>
+  </si>
+  <si>
+    <t>51482133</t>
+  </si>
+  <si>
+    <t>51482134</t>
+  </si>
+  <si>
+    <t>51482135</t>
+  </si>
+  <si>
+    <t>51482136</t>
+  </si>
+  <si>
+    <t>51482302</t>
+  </si>
+  <si>
+    <t>51482309</t>
+  </si>
+  <si>
+    <t>51482311</t>
+  </si>
+  <si>
+    <t>51482313</t>
+  </si>
+  <si>
+    <t>51482331</t>
+  </si>
+  <si>
+    <t>51482333</t>
+  </si>
+  <si>
+    <t>51482336</t>
+  </si>
+  <si>
+    <t>51482339</t>
+  </si>
+  <si>
+    <t>51482342</t>
+  </si>
+  <si>
+    <t>51482345</t>
+  </si>
+  <si>
+    <t>51482348</t>
+  </si>
+  <si>
+    <t>51482351</t>
+  </si>
+  <si>
+    <t>51482354</t>
+  </si>
+  <si>
+    <t>51482355</t>
+  </si>
+  <si>
+    <t>51482356</t>
+  </si>
+  <si>
+    <t>51482357</t>
+  </si>
+  <si>
+    <t>51482360</t>
   </si>
 </sst>
 </file>
@@ -765,7 +846,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="169">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -830,6 +911,85 @@
     <xf applyBorder="1" applyFill="1" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="15" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
@@ -1480,7 +1640,7 @@
       <c r="Q2" s="59">
         <v>1</v>
       </c>
-      <c r="R2" s="89" t="s">
+      <c r="R2" s="141" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1530,7 +1690,7 @@
       <c r="Q3" s="59">
         <v>1</v>
       </c>
-      <c r="R3" s="80" t="s">
+      <c r="R3" s="144" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1583,7 +1743,7 @@
       <c r="Q4" s="59">
         <v>1</v>
       </c>
-      <c r="R4" s="83" t="s">
+      <c r="R4" s="147" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1639,7 +1799,7 @@
       <c r="Q5" s="59">
         <v>1</v>
       </c>
-      <c r="R5" s="86" t="s">
+      <c r="R5" s="150" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1692,7 +1852,7 @@
       <c r="Q6" s="59">
         <v>1</v>
       </c>
-      <c r="R6" s="88" t="s">
+      <c r="R6" s="153" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1726,7 +1886,7 @@
       <c r="Q7" s="59">
         <v>1</v>
       </c>
-      <c r="R7" s="49" t="s">
+      <c r="R7" s="156" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1779,8 +1939,8 @@
       <c r="Q8" s="59">
         <v>1</v>
       </c>
-      <c r="R8" s="50" t="s">
-        <v>148</v>
+      <c r="R8" s="158" t="s">
+        <v>179</v>
       </c>
       <c r="S8" s="45"/>
     </row>
@@ -1833,8 +1993,8 @@
       <c r="Q9" s="59">
         <v>1</v>
       </c>
-      <c r="R9" s="51" t="s">
-        <v>149</v>
+      <c r="R9" s="160" t="s">
+        <v>180</v>
       </c>
       <c r="S9" s="15"/>
     </row>
@@ -1888,8 +2048,8 @@
       <c r="Q10" s="59">
         <v>1</v>
       </c>
-      <c r="R10" s="52" t="s">
-        <v>150</v>
+      <c r="R10" s="162" t="s">
+        <v>181</v>
       </c>
     </row>
     <row customFormat="1" r="11" s="6" spans="1:19">
@@ -1941,7 +2101,7 @@
       <c r="Q11" s="59">
         <v>1</v>
       </c>
-      <c r="R11" s="53" t="s">
+      <c r="R11" s="165" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1975,7 +2135,7 @@
       <c r="Q12" s="59">
         <v>1</v>
       </c>
-      <c r="R12" s="54" t="s">
+      <c r="R12" s="168" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Addition of overage tests
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/FCFile.xlsx
+++ b/binaries/FCfiles/FCFile.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="222">
   <si>
     <t>shipmentType</t>
   </si>
@@ -596,6 +596,120 @@
   </si>
   <si>
     <t>51482360</t>
+  </si>
+  <si>
+    <t>51483175</t>
+  </si>
+  <si>
+    <t>51483183</t>
+  </si>
+  <si>
+    <t>51483189</t>
+  </si>
+  <si>
+    <t>51483193</t>
+  </si>
+  <si>
+    <t>51483197</t>
+  </si>
+  <si>
+    <t>51483200</t>
+  </si>
+  <si>
+    <t>51483201</t>
+  </si>
+  <si>
+    <t>51483202</t>
+  </si>
+  <si>
+    <t>51483203</t>
+  </si>
+  <si>
+    <t>51483211</t>
+  </si>
+  <si>
+    <t>51483927</t>
+  </si>
+  <si>
+    <t>51483931</t>
+  </si>
+  <si>
+    <t>51483936</t>
+  </si>
+  <si>
+    <t>51483942</t>
+  </si>
+  <si>
+    <t>51483945</t>
+  </si>
+  <si>
+    <t>51483950</t>
+  </si>
+  <si>
+    <t>51483951</t>
+  </si>
+  <si>
+    <t>51483954</t>
+  </si>
+  <si>
+    <t>51484520</t>
+  </si>
+  <si>
+    <t>51484531</t>
+  </si>
+  <si>
+    <t>51484532</t>
+  </si>
+  <si>
+    <t>51484534</t>
+  </si>
+  <si>
+    <t>51484586</t>
+  </si>
+  <si>
+    <t>51484866</t>
+  </si>
+  <si>
+    <t>51484868</t>
+  </si>
+  <si>
+    <t>51484870</t>
+  </si>
+  <si>
+    <t>51484872</t>
+  </si>
+  <si>
+    <t>51484874</t>
+  </si>
+  <si>
+    <t>51484876</t>
+  </si>
+  <si>
+    <t>51484877</t>
+  </si>
+  <si>
+    <t>51484897</t>
+  </si>
+  <si>
+    <t>51484899</t>
+  </si>
+  <si>
+    <t>51484901</t>
+  </si>
+  <si>
+    <t>51484903</t>
+  </si>
+  <si>
+    <t>51484905</t>
+  </si>
+  <si>
+    <t>51484908</t>
+  </si>
+  <si>
+    <t>51484909</t>
+  </si>
+  <si>
+    <t>51484911</t>
   </si>
 </sst>
 </file>
@@ -846,7 +960,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="274">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -911,6 +1025,111 @@
     <xf applyBorder="1" applyFill="1" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="15" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="15" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="17" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
@@ -1640,8 +1859,8 @@
       <c r="Q2" s="59">
         <v>1</v>
       </c>
-      <c r="R2" s="141" t="s">
-        <v>83</v>
+      <c r="R2" s="256" t="s">
+        <v>214</v>
       </c>
     </row>
     <row customFormat="1" r="3" s="6" spans="1:19">
@@ -1690,7 +1909,7 @@
       <c r="Q3" s="59">
         <v>1</v>
       </c>
-      <c r="R3" s="144" t="s">
+      <c r="R3" s="257" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1743,8 +1962,8 @@
       <c r="Q4" s="59">
         <v>1</v>
       </c>
-      <c r="R4" s="147" t="s">
-        <v>83</v>
+      <c r="R4" s="260" t="s">
+        <v>216</v>
       </c>
     </row>
     <row customFormat="1" r="5" s="6" spans="1:19">
@@ -1799,7 +2018,7 @@
       <c r="Q5" s="59">
         <v>1</v>
       </c>
-      <c r="R5" s="150" t="s">
+      <c r="R5" s="261" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1852,8 +2071,8 @@
       <c r="Q6" s="59">
         <v>1</v>
       </c>
-      <c r="R6" s="153" t="s">
-        <v>83</v>
+      <c r="R6" s="264" t="s">
+        <v>218</v>
       </c>
     </row>
     <row customFormat="1" r="7" s="6" spans="1:19">
@@ -1886,7 +2105,7 @@
       <c r="Q7" s="59">
         <v>1</v>
       </c>
-      <c r="R7" s="156" t="s">
+      <c r="R7" s="265" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1939,8 +2158,8 @@
       <c r="Q8" s="59">
         <v>1</v>
       </c>
-      <c r="R8" s="158" t="s">
-        <v>179</v>
+      <c r="R8" s="266" t="s">
+        <v>83</v>
       </c>
       <c r="S8" s="45"/>
     </row>
@@ -1993,8 +2212,8 @@
       <c r="Q9" s="59">
         <v>1</v>
       </c>
-      <c r="R9" s="160" t="s">
-        <v>180</v>
+      <c r="R9" s="267" t="s">
+        <v>83</v>
       </c>
       <c r="S9" s="15"/>
     </row>
@@ -2048,8 +2267,8 @@
       <c r="Q10" s="59">
         <v>1</v>
       </c>
-      <c r="R10" s="162" t="s">
-        <v>181</v>
+      <c r="R10" s="269" t="s">
+        <v>219</v>
       </c>
     </row>
     <row customFormat="1" r="11" s="6" spans="1:19">
@@ -2101,8 +2320,8 @@
       <c r="Q11" s="59">
         <v>1</v>
       </c>
-      <c r="R11" s="165" t="s">
-        <v>83</v>
+      <c r="R11" s="272" t="s">
+        <v>221</v>
       </c>
     </row>
     <row customFormat="1" r="12" s="6" spans="1:19">
@@ -2135,7 +2354,7 @@
       <c r="Q12" s="59">
         <v>1</v>
       </c>
-      <c r="R12" s="168" t="s">
+      <c r="R12" s="273" t="s">
         <v>83</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Addition of Manage Claims, Sign Up and Forgot Password
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/FCFile.xlsx
+++ b/binaries/FCfiles/FCFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charu\eclipse-workspace\qualitesoft\binaries\FCfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SONY\git\qualitesoft\binaries\FCfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{7481207D-8925-4522-90E7-018C8D0EFD08}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{D4EE8EFF-0047-4117-844C-280533D4FD20}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="2" tabRatio="449" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
+    <workbookView activeTab="2" tabRatio="449" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="CreateAccount" r:id="rId1" sheetId="5"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="165">
   <si>
     <t>shipmentType</t>
   </si>
@@ -414,39 +414,6 @@
     <t>Test Pallet Description</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>51487037</t>
-  </si>
-  <si>
-    <t>51487040</t>
-  </si>
-  <si>
-    <t>51487043</t>
-  </si>
-  <si>
-    <t>51487044</t>
-  </si>
-  <si>
-    <t>51487047</t>
-  </si>
-  <si>
-    <t>51487050</t>
-  </si>
-  <si>
-    <t>51487051</t>
-  </si>
-  <si>
-    <t>51487053</t>
-  </si>
-  <si>
-    <t>51487056</t>
-  </si>
-  <si>
-    <t>51487059</t>
-  </si>
-  <si>
     <t>Standard Pallet 1</t>
   </si>
   <si>
@@ -519,27 +486,18 @@
     <t>Ceva</t>
   </si>
   <si>
-    <t>51487599</t>
-  </si>
-  <si>
     <t>$1,044.52</t>
   </si>
   <si>
     <t>07-18-2021</t>
   </si>
   <si>
-    <t>51487601</t>
-  </si>
-  <si>
     <t>NPSKU</t>
   </si>
   <si>
     <t>PSKU</t>
   </si>
   <si>
-    <t>51487602</t>
-  </si>
-  <si>
     <t>$1,055.50</t>
   </si>
   <si>
@@ -552,7 +510,19 @@
     <t>New Product</t>
   </si>
   <si>
-    <t>51487615</t>
+    <t>600</t>
+  </si>
+  <si>
+    <t>07-27-2021</t>
+  </si>
+  <si>
+    <t>51489386</t>
+  </si>
+  <si>
+    <t>08-07-2021</t>
+  </si>
+  <si>
+    <t>51489387</t>
   </si>
 </sst>
 </file>
@@ -576,7 +546,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="47">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -726,6 +696,31 @@
       </patternFill>
     </fill>
     <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
       <patternFill patternType="none">
         <fgColor indexed="9"/>
       </patternFill>
@@ -755,8 +750,38 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="28">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -998,6 +1023,71 @@
         <color auto="1"/>
       </bottom>
       <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
     <border>
       <top style="thin"/>
@@ -1028,7 +1118,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="83">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -1085,25 +1175,33 @@
     <xf applyBorder="1" applyFill="1" borderId="1" fillId="19" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="18" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="11" fillId="20" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="12" fillId="20" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="19" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="13" fillId="21" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="14" fillId="22" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="15" fillId="23" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="16" fillId="24" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="17" fillId="25" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="18" fillId="26" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="19" fillId="27" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="20" fillId="28" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="21" fillId="29" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="21" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="21" fillId="20" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="12" fillId="21" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="13" fillId="22" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="14" fillId="23" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="15" fillId="24" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="16" fillId="25" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="17" fillId="26" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="17" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="17" fillId="20" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="4" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="23" fillId="31" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="25" fillId="33" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="27" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="1" applyFill="1" borderId="18" fillId="27" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="19" fillId="28" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="20" fillId="29" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="10" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="21" fillId="30" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="22" fillId="31" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="23" fillId="32" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="24" fillId="33" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="25" fillId="34" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="27" fillId="36" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="29" fillId="38" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="31" fillId="40" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="33" fillId="42" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="35" fillId="44" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="37" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -1388,23 +1486,23 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.88671875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="27.109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.44140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.6640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="40" width="14.109375" collapsed="true"/>
-    <col min="9" max="9" style="40" width="9.109375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="40" width="14.140625" collapsed="true"/>
+    <col min="9" max="9" style="40" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -1433,7 +1531,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -1447,7 +1545,7 @@
         <v>77</v>
       </c>
       <c r="E2" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="F2" t="s">
         <v>79</v>
@@ -1456,7 +1554,7 @@
         <v>79</v>
       </c>
       <c r="H2" s="40" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="I2" s="40" t="s">
         <v>78</v>
@@ -1470,23 +1568,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.44140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.33203125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
     <col min="15" max="15" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="13.88671875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="19.33203125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -1544,8 +1642,11 @@
       <c r="S1" t="s">
         <v>101</v>
       </c>
+      <c r="T1" s="3" t="s">
+        <v>125</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -1602,6 +1703,9 @@
       </c>
       <c r="S2" s="40" t="s">
         <v>110</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1616,41 +1720,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2:S18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="17.5546875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="17.5703125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="11.43359375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="31.109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="31.140625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="17.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="9.6640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="11.33203125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="10.6640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="12.33203125" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" style="1" width="33.44140625" collapsed="true"/>
-    <col min="11" max="13" style="1" width="9.109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="11.88671875" collapsed="true"/>
-    <col min="15" max="15" style="1" width="9.109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.109375" collapsed="true"/>
-    <col min="17" max="18" style="1" width="9.109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="11.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
+    <col min="9" max="10" customWidth="true" style="1" width="33.42578125" collapsed="true"/>
+    <col min="11" max="13" style="1" width="9.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="11.85546875" collapsed="true"/>
+    <col min="15" max="15" style="1" width="9.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
+    <col min="17" max="18" style="1" width="9.140625" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="9.95703125" collapsed="true"/>
     <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="9.9453125" collapsed="true"/>
     <col min="21" max="21" customWidth="true" style="1" width="10.0" collapsed="true"/>
     <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="19.33203125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="17.21875" collapsed="true"/>
-    <col min="25" max="16384" style="1" width="9.109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="25" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -1703,11 +1807,11 @@
       <c r="S1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="T1" s="57" t="s">
-        <v>149</v>
-      </c>
-      <c r="U1" s="57" t="s">
-        <v>161</v>
+      <c r="T1" s="56" t="s">
+        <v>138</v>
+      </c>
+      <c r="U1" s="56" t="s">
+        <v>150</v>
       </c>
       <c r="V1" s="3" t="s">
         <v>124</v>
@@ -1716,10 +1820,10 @@
         <v>125</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15.75" r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -1754,11 +1858,9 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="S2" s="42" t="s">
-        <v>129</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="S2" s="75"/>
       <c r="T2" s="42"/>
       <c r="U2" s="42"/>
       <c r="V2" s="3" t="s">
@@ -1767,7 +1869,7 @@
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -1797,12 +1899,12 @@
         <v>63</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>18</v>
@@ -1811,14 +1913,12 @@
         <v>122</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="S3" s="43" t="s">
         <v>130</v>
       </c>
+      <c r="S3" s="43"/>
       <c r="T3" s="43"/>
       <c r="U3" s="43"/>
       <c r="V3" s="3" t="s">
@@ -1827,7 +1927,7 @@
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
     </row>
-    <row customHeight="1" ht="15.75" r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15.75" r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -1855,41 +1955,41 @@
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>122</v>
+        <v>160</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="S4" s="44" t="s">
-        <v>131</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="S4" s="71"/>
       <c r="T4" s="44"/>
-      <c r="U4" s="44"/>
+      <c r="U4" s="44" t="s">
+        <v>151</v>
+      </c>
       <c r="V4" s="3" t="s">
         <v>126</v>
       </c>
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -1919,16 +2019,16 @@
         <v>20</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>18</v>
@@ -1937,23 +2037,21 @@
         <v>122</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="S5" s="45" t="s">
-        <v>132</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="S5" s="45"/>
       <c r="T5" s="45"/>
       <c r="U5" s="45"/>
       <c r="V5" s="3" t="s">
-        <v>126</v>
+        <v>64</v>
       </c>
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
@@ -1981,16 +2079,16 @@
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="N6" s="59" t="s">
-        <v>158</v>
+        <v>145</v>
+      </c>
+      <c r="N6" s="58" t="s">
+        <v>147</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>18</v>
@@ -1999,14 +2097,12 @@
         <v>122</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="S6" s="46" t="s">
-        <v>133</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="S6" s="46"/>
       <c r="T6" s="46"/>
       <c r="U6" s="46"/>
       <c r="V6" s="3" t="s">
@@ -2015,7 +2111,7 @@
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -2050,11 +2146,9 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="S7" s="47" t="s">
-        <v>134</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="S7" s="47"/>
       <c r="T7" s="47"/>
       <c r="U7" s="47"/>
       <c r="V7" s="3" t="s">
@@ -2063,7 +2157,7 @@
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
@@ -2091,16 +2185,16 @@
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>18</v>
@@ -2109,14 +2203,12 @@
         <v>122</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="S8" s="48" t="s">
-        <v>135</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="S8" s="48"/>
       <c r="T8" s="48"/>
       <c r="U8" s="48"/>
       <c r="V8" s="3" t="s">
@@ -2125,7 +2217,7 @@
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
@@ -2153,16 +2245,16 @@
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="O9" s="3" t="s">
         <v>18</v>
@@ -2171,14 +2263,12 @@
         <v>122</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="S9" s="49" t="s">
-        <v>128</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="S9" s="76"/>
       <c r="T9" s="49"/>
       <c r="U9" s="49"/>
       <c r="V9" s="3" t="s">
@@ -2187,7 +2277,7 @@
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -2215,16 +2305,16 @@
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="M10" s="59" t="s">
-        <v>151</v>
-      </c>
-      <c r="N10" s="59" t="s">
-        <v>158</v>
+        <v>140</v>
+      </c>
+      <c r="M10" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="N10" s="58" t="s">
+        <v>147</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>18</v>
@@ -2233,14 +2323,12 @@
         <v>122</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="S10" s="50" t="s">
-        <v>136</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="S10" s="50"/>
       <c r="T10" s="50"/>
       <c r="U10" s="50"/>
       <c r="V10" s="3" t="s">
@@ -2249,7 +2337,7 @@
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -2277,16 +2365,16 @@
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="N11" s="59" t="s">
-        <v>158</v>
+        <v>146</v>
+      </c>
+      <c r="N11" s="58" t="s">
+        <v>147</v>
       </c>
       <c r="O11" s="3" t="s">
         <v>18</v>
@@ -2295,14 +2383,12 @@
         <v>122</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="S11" s="51" t="s">
-        <v>137</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="S11" s="51"/>
       <c r="T11" s="51"/>
       <c r="U11" s="51"/>
       <c r="V11" s="3" t="s">
@@ -2311,7 +2397,7 @@
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -2346,11 +2432,9 @@
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
       <c r="R12" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="S12" s="52" t="s">
-        <v>138</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="S12" s="52"/>
       <c r="T12" s="52"/>
       <c r="U12" s="52"/>
       <c r="V12" s="3" t="s">
@@ -2359,18 +2443,18 @@
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B13" s="61" t="s">
-        <v>165</v>
+        <v>135</v>
+      </c>
+      <c r="B13" s="81" t="s">
+        <v>163</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>26</v>
@@ -2385,20 +2469,20 @@
         <v>16</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="2" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="O13" s="3" t="s">
         <v>18</v>
@@ -2407,19 +2491,19 @@
         <v>122</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="S13" s="60" t="s">
-        <v>163</v>
-      </c>
-      <c r="T13" s="62" t="s">
+        <v>130</v>
+      </c>
+      <c r="S13" s="80" t="s">
         <v>164</v>
       </c>
-      <c r="U13" s="58" t="s">
-        <v>162</v>
+      <c r="T13" s="82" t="s">
+        <v>152</v>
+      </c>
+      <c r="U13" s="57" t="s">
+        <v>151</v>
       </c>
       <c r="V13" s="3" t="s">
         <v>126</v>
@@ -2428,21 +2512,21 @@
         <v>127</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B14" s="64" t="s">
-        <v>165</v>
+        <v>135</v>
+      </c>
+      <c r="B14" s="60" t="s">
+        <v>153</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>26</v>
@@ -2457,20 +2541,20 @@
         <v>16</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="2" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="O14" s="3" t="s">
         <v>18</v>
@@ -2479,29 +2563,27 @@
         <v>122</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="S14" s="63" t="s">
-        <v>166</v>
-      </c>
-      <c r="T14" s="65" t="s">
-        <v>164</v>
+        <v>130</v>
+      </c>
+      <c r="S14" s="59"/>
+      <c r="T14" s="61" t="s">
+        <v>152</v>
       </c>
       <c r="U14" s="53" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="V14" s="3" t="s">
         <v>64</v>
       </c>
       <c r="W14" s="3"/>
       <c r="X14" s="2" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2515,16 +2597,16 @@
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="2" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>18</v>
@@ -2533,10 +2615,10 @@
         <v>122</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="S15" s="54"/>
       <c r="T15" s="54"/>
@@ -2547,18 +2629,18 @@
       <c r="W15" s="3"/>
       <c r="X15" s="2"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B16" s="73" t="s">
-        <v>165</v>
+        <v>135</v>
+      </c>
+      <c r="B16" s="69" t="s">
+        <v>153</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>26</v>
@@ -2573,20 +2655,20 @@
         <v>16</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="2" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="O16" s="3" t="s">
         <v>18</v>
@@ -2595,31 +2677,29 @@
         <v>122</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="S16" s="72" t="s">
-        <v>174</v>
-      </c>
-      <c r="T16" s="74" t="s">
-        <v>164</v>
-      </c>
-      <c r="U16" s="56" t="s">
-        <v>162</v>
+        <v>130</v>
+      </c>
+      <c r="S16" s="68"/>
+      <c r="T16" s="70" t="s">
+        <v>152</v>
+      </c>
+      <c r="U16" s="55" t="s">
+        <v>151</v>
       </c>
       <c r="V16" s="3" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="W16" s="3"/>
       <c r="X16" s="2" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="69"/>
+      <c r="B17" s="65"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="2"/>
@@ -2629,16 +2709,16 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="40" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="L17" s="40" t="s">
-        <v>172</v>
-      </c>
-      <c r="M17" s="71" t="s">
-        <v>151</v>
-      </c>
-      <c r="N17" s="71" t="s">
-        <v>151</v>
+        <v>158</v>
+      </c>
+      <c r="M17" s="67" t="s">
+        <v>140</v>
+      </c>
+      <c r="N17" s="67" t="s">
+        <v>140</v>
       </c>
       <c r="O17" s="3" t="s">
         <v>18</v>
@@ -2648,27 +2728,27 @@
       </c>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
-      <c r="S17" s="70"/>
-      <c r="T17" s="70"/>
-      <c r="U17" s="70"/>
+      <c r="S17" s="66"/>
+      <c r="T17" s="66"/>
+      <c r="U17" s="66"/>
       <c r="V17" s="3" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="W17" s="3"/>
       <c r="X17" s="2"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B18" s="67" t="s">
-        <v>165</v>
+        <v>135</v>
+      </c>
+      <c r="B18" s="63" t="s">
+        <v>153</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>26</v>
@@ -2687,40 +2767,38 @@
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="2" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="O18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="Q18" s="3"/>
       <c r="R18" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="S18" s="66" t="s">
-        <v>169</v>
-      </c>
-      <c r="T18" s="68" t="s">
-        <v>170</v>
-      </c>
-      <c r="U18" s="56" t="s">
-        <v>162</v>
+        <v>130</v>
+      </c>
+      <c r="S18" s="62"/>
+      <c r="T18" s="64" t="s">
+        <v>156</v>
+      </c>
+      <c r="U18" s="55" t="s">
+        <v>151</v>
       </c>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
       <c r="X18" s="2" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2737,35 +2815,35 @@
       <selection activeCell="AC7" sqref="AC7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.6640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.44140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.88671875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="7.6640625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
     <col min="16" max="16" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="19.44140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="11.109375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="9.33203125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2848,7 +2926,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -2919,7 +2997,7 @@
       <c r="Z2" s="11"/>
       <c r="AA2" s="19"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>22</v>
       </c>
@@ -2989,7 +3067,7 @@
       <c r="Y3" s="20"/>
       <c r="Z3" s="12"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>22</v>
       </c>
@@ -3059,7 +3137,7 @@
       <c r="Y4" s="20"/>
       <c r="Z4" s="13"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>22</v>
       </c>
@@ -3129,7 +3207,7 @@
       <c r="Y5" s="20"/>
       <c r="Z5" s="14"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
@@ -3199,7 +3277,7 @@
       <c r="Y6" s="20"/>
       <c r="Z6" s="15"/>
     </row>
-    <row customFormat="1" r="7" s="33" spans="1:27" x14ac:dyDescent="0.3">
+    <row customFormat="1" r="7" s="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>22</v>
       </c>
@@ -3268,7 +3346,7 @@
       <c r="X7" s="39"/>
       <c r="Y7" s="39"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
@@ -3340,7 +3418,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -3412,7 +3490,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -3490,7 +3568,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
@@ -3559,7 +3637,7 @@
       <c r="X11" s="21"/>
       <c r="Y11" s="21"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -3628,7 +3706,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
@@ -3697,7 +3775,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Addition of Demo xml
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/FCFile.xlsx
+++ b/binaries/FCfiles/FCFile.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="176">
   <si>
     <t>shipmentType</t>
   </si>
@@ -523,6 +523,39 @@
   </si>
   <si>
     <t>51489387</t>
+  </si>
+  <si>
+    <t>51490045</t>
+  </si>
+  <si>
+    <t>08-16-2021</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>51490054</t>
+  </si>
+  <si>
+    <t>51490057</t>
+  </si>
+  <si>
+    <t>51490061</t>
+  </si>
+  <si>
+    <t>51490066</t>
+  </si>
+  <si>
+    <t>51490078</t>
+  </si>
+  <si>
+    <t>51490081</t>
+  </si>
+  <si>
+    <t>51490257</t>
+  </si>
+  <si>
+    <t>51490259</t>
   </si>
 </sst>
 </file>
@@ -546,7 +579,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="47">
+  <fills count="95">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -780,8 +813,248 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="38">
+  <borders count="86">
     <border>
       <left/>
       <right/>
@@ -1110,6 +1383,174 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
@@ -1118,7 +1559,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="107">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -1201,7 +1642,31 @@
     <xf applyBorder="true" applyFill="true" borderId="31" fillId="40" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="33" fillId="42" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="35" fillId="44" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="37" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="37" fillId="46" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="39" fillId="48" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="41" fillId="50" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="43" fillId="52" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="45" fillId="54" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="47" fillId="56" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="49" fillId="58" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="51" fillId="60" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="53" fillId="62" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="55" fillId="64" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="57" fillId="66" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="59" fillId="68" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="61" fillId="70" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="63" fillId="72" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="65" fillId="74" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="67" fillId="76" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="69" fillId="78" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="71" fillId="80" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="73" fillId="82" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="75" fillId="84" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="77" fillId="86" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="79" fillId="88" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="81" fillId="90" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="83" fillId="92" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="94" borderId="85" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -1860,7 +2325,9 @@
       <c r="R2" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S2" s="75"/>
+      <c r="S2" s="103" t="s">
+        <v>167</v>
+      </c>
       <c r="T2" s="42"/>
       <c r="U2" s="42"/>
       <c r="V2" s="3" t="s">
@@ -1918,7 +2385,9 @@
       <c r="R3" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S3" s="43"/>
+      <c r="S3" s="89" t="s">
+        <v>169</v>
+      </c>
       <c r="T3" s="43"/>
       <c r="U3" s="43"/>
       <c r="V3" s="3" t="s">
@@ -1978,7 +2447,9 @@
       <c r="R4" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S4" s="71"/>
+      <c r="S4" s="106" t="s">
+        <v>175</v>
+      </c>
       <c r="T4" s="44"/>
       <c r="U4" s="44" t="s">
         <v>151</v>
@@ -2042,7 +2513,9 @@
       <c r="R5" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S5" s="45"/>
+      <c r="S5" s="93" t="s">
+        <v>171</v>
+      </c>
       <c r="T5" s="45"/>
       <c r="U5" s="45"/>
       <c r="V5" s="3" t="s">
@@ -2102,7 +2575,9 @@
       <c r="R6" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S6" s="46"/>
+      <c r="S6" s="94" t="s">
+        <v>167</v>
+      </c>
       <c r="T6" s="46"/>
       <c r="U6" s="46"/>
       <c r="V6" s="3" t="s">
@@ -2148,7 +2623,9 @@
       <c r="R7" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S7" s="47"/>
+      <c r="S7" s="95" t="s">
+        <v>167</v>
+      </c>
       <c r="T7" s="47"/>
       <c r="U7" s="47"/>
       <c r="V7" s="3" t="s">
@@ -2208,7 +2685,9 @@
       <c r="R8" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S8" s="48"/>
+      <c r="S8" s="97" t="s">
+        <v>172</v>
+      </c>
       <c r="T8" s="48"/>
       <c r="U8" s="48"/>
       <c r="V8" s="3" t="s">
@@ -2268,7 +2747,9 @@
       <c r="R9" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S9" s="76"/>
+      <c r="S9" s="99" t="s">
+        <v>173</v>
+      </c>
       <c r="T9" s="49"/>
       <c r="U9" s="49"/>
       <c r="V9" s="3" t="s">
@@ -2328,7 +2809,9 @@
       <c r="R10" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S10" s="50"/>
+      <c r="S10" s="100" t="s">
+        <v>167</v>
+      </c>
       <c r="T10" s="50"/>
       <c r="U10" s="50"/>
       <c r="V10" s="3" t="s">
@@ -2388,7 +2871,9 @@
       <c r="R11" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S11" s="51"/>
+      <c r="S11" s="101" t="s">
+        <v>167</v>
+      </c>
       <c r="T11" s="51"/>
       <c r="U11" s="51"/>
       <c r="V11" s="3" t="s">
@@ -2434,7 +2919,9 @@
       <c r="R12" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S12" s="52"/>
+      <c r="S12" s="102" t="s">
+        <v>167</v>
+      </c>
       <c r="T12" s="52"/>
       <c r="U12" s="52"/>
       <c r="V12" s="3" t="s">
@@ -2633,8 +3120,8 @@
       <c r="A16" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B16" s="69" t="s">
-        <v>153</v>
+      <c r="B16" s="84" t="s">
+        <v>166</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>19</v>
@@ -2682,8 +3169,10 @@
       <c r="R16" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S16" s="68"/>
-      <c r="T16" s="70" t="s">
+      <c r="S16" s="83" t="s">
+        <v>165</v>
+      </c>
+      <c r="T16" s="85" t="s">
         <v>152</v>
       </c>
       <c r="U16" s="55" t="s">

</xml_diff>

<commit_message>
Fixed demo scripts issue.
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/FCFile.xlsx
+++ b/binaries/FCfiles/FCFile.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SONY\git\qualitesoft\binaries\FCfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{D4EE8EFF-0047-4117-844C-280533D4FD20}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7BCCD6-729B-4573-A6CA-2BE1F3EA437F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="2" tabRatio="449" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="449" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CreateAccount" r:id="rId1" sheetId="5"/>
-    <sheet name="ShipmentInformation" r:id="rId2" sheetId="6"/>
-    <sheet name="Input" r:id="rId3" sheetId="1"/>
-    <sheet name="Marrkups" r:id="rId4" sheetId="4"/>
+    <sheet name="CreateAccount" sheetId="5" r:id="rId1"/>
+    <sheet name="ShipmentInformation" sheetId="6" r:id="rId2"/>
+    <sheet name="Input" sheetId="1" r:id="rId3"/>
+    <sheet name="Marrkups" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="166">
   <si>
     <t>shipmentType</t>
   </si>
@@ -489,18 +489,12 @@
     <t>$1,044.52</t>
   </si>
   <si>
-    <t>07-18-2021</t>
-  </si>
-  <si>
     <t>NPSKU</t>
   </si>
   <si>
     <t>PSKU</t>
   </si>
   <si>
-    <t>$1,055.50</t>
-  </si>
-  <si>
     <t>400</t>
   </si>
   <si>
@@ -513,62 +507,31 @@
     <t>600</t>
   </si>
   <si>
-    <t>07-27-2021</t>
-  </si>
-  <si>
-    <t>51489386</t>
-  </si>
-  <si>
-    <t>08-07-2021</t>
-  </si>
-  <si>
-    <t>51489387</t>
-  </si>
-  <si>
-    <t>51490045</t>
-  </si>
-  <si>
-    <t>08-16-2021</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>51490054</t>
-  </si>
-  <si>
-    <t>51490057</t>
-  </si>
-  <si>
-    <t>51490061</t>
-  </si>
-  <si>
-    <t>51490066</t>
-  </si>
-  <si>
-    <t>51490078</t>
-  </si>
-  <si>
-    <t>51490081</t>
-  </si>
-  <si>
-    <t>51490257</t>
-  </si>
-  <si>
-    <t>51490259</t>
-  </si>
-  <si>
-    <t>51490872</t>
-  </si>
-  <si>
-    <t>51490874</t>
+    <t>08-23-2021</t>
+  </si>
+  <si>
+    <t>51490953</t>
+  </si>
+  <si>
+    <t>51490956</t>
+  </si>
+  <si>
+    <t>51490965</t>
+  </si>
+  <si>
+    <t>51490966</t>
+  </si>
+  <si>
+    <t>$727.51</t>
+  </si>
+  <si>
+    <t>51491260</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -585,7 +548,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="105">
+  <fills count="47">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -760,347 +723,57 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
@@ -1110,7 +783,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="96">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1398,378 +1071,241 @@
       <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="112">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="3" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="4" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="4" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="5" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="6" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="7" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="7" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="7" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="8" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="9" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="10" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="6" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="5" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="8" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="13" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="14" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="15" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="16" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="17" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="19" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="18" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="11" fillId="20" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="19" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="12" fillId="21" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="13" fillId="22" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="14" fillId="23" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="15" fillId="24" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="16" fillId="25" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="17" fillId="26" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="17" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="17" fillId="20" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="4" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="18" fillId="27" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="19" fillId="28" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="20" fillId="29" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="10" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="21" fillId="30" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="22" fillId="31" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="23" fillId="32" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="24" fillId="33" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="25" fillId="34" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="27" fillId="36" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="29" fillId="38" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="31" fillId="40" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="33" fillId="42" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="35" fillId="44" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="37" fillId="46" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="39" fillId="48" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="41" fillId="50" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="43" fillId="52" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="45" fillId="54" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="47" fillId="56" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="49" fillId="58" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="51" fillId="60" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="53" fillId="62" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="55" fillId="64" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="57" fillId="66" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="59" fillId="68" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="61" fillId="70" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="63" fillId="72" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="65" fillId="74" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="67" fillId="76" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="69" fillId="78" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="71" fillId="80" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="73" fillId="82" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="75" fillId="84" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="77" fillId="86" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="79" fillId="88" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="81" fillId="90" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="83" fillId="92" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="85" fillId="94" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="87" fillId="96" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="89" fillId="98" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="91" fillId="100" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="93" fillId="102" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="104" borderId="95" xfId="0" applyFill="true" applyBorder="true"/>
+  <cellXfs count="88">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1786,10 +1322,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1953,21 +1489,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1984,7 +1520,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2036,15 +1572,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2052,15 +1588,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="40" width="14.140625" collapsed="true"/>
-    <col min="9" max="9" style="40" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.140625" style="40" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="40" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2122,13 +1658,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -2137,12 +1673,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -2271,43 +1807,42 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="I2" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Y18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:X19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S18"/>
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="11.43359375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="31.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="17.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="11.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" style="1" width="33.42578125" collapsed="true"/>
-    <col min="11" max="13" style="1" width="9.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="11.85546875" collapsed="true"/>
-    <col min="15" max="15" style="1" width="9.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="17" max="18" style="1" width="9.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="9.95703125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="9.9453125" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="25" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="31.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="33.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="13" width="9.140625" style="1" collapsed="1"/>
+    <col min="14" max="14" width="11.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="9.140625" style="1" collapsed="1"/>
+    <col min="16" max="16" width="14.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="18" width="9.140625" style="1" collapsed="1"/>
+    <col min="19" max="20" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10" style="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="19.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
@@ -2384,7 +1919,7 @@
         <v>129</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -2421,9 +1956,7 @@
       <c r="R2" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S2" s="103" t="s">
-        <v>167</v>
-      </c>
+      <c r="S2" s="73"/>
       <c r="T2" s="42"/>
       <c r="U2" s="42"/>
       <c r="V2" s="3" t="s">
@@ -2481,9 +2014,7 @@
       <c r="R3" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S3" s="89" t="s">
-        <v>169</v>
-      </c>
+      <c r="S3" s="64"/>
       <c r="T3" s="43"/>
       <c r="U3" s="43"/>
       <c r="V3" s="3" t="s">
@@ -2492,7 +2023,7 @@
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
     </row>
-    <row customHeight="1" ht="15.75" r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -2535,7 +2066,7 @@
         <v>18</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>130</v>
@@ -2543,8 +2074,8 @@
       <c r="R4" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S4" s="111" t="s">
-        <v>177</v>
+      <c r="S4" s="87" t="s">
+        <v>165</v>
       </c>
       <c r="T4" s="44"/>
       <c r="U4" s="44" t="s">
@@ -2554,7 +2085,9 @@
         <v>126</v>
       </c>
       <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
+      <c r="X4" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -2609,9 +2142,7 @@
       <c r="R5" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S5" s="93" t="s">
-        <v>171</v>
-      </c>
+      <c r="S5" s="65"/>
       <c r="T5" s="45"/>
       <c r="U5" s="45"/>
       <c r="V5" s="3" t="s">
@@ -2671,9 +2202,7 @@
       <c r="R6" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S6" s="94" t="s">
-        <v>167</v>
-      </c>
+      <c r="S6" s="66"/>
       <c r="T6" s="46"/>
       <c r="U6" s="46"/>
       <c r="V6" s="3" t="s">
@@ -2719,9 +2248,7 @@
       <c r="R7" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S7" s="95" t="s">
-        <v>167</v>
-      </c>
+      <c r="S7" s="67"/>
       <c r="T7" s="47"/>
       <c r="U7" s="47"/>
       <c r="V7" s="3" t="s">
@@ -2781,9 +2308,7 @@
       <c r="R8" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S8" s="97" t="s">
-        <v>172</v>
-      </c>
+      <c r="S8" s="68"/>
       <c r="T8" s="48"/>
       <c r="U8" s="48"/>
       <c r="V8" s="3" t="s">
@@ -2843,9 +2368,7 @@
       <c r="R9" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S9" s="99" t="s">
-        <v>173</v>
-      </c>
+      <c r="S9" s="69"/>
       <c r="T9" s="49"/>
       <c r="U9" s="49"/>
       <c r="V9" s="3" t="s">
@@ -2905,9 +2428,7 @@
       <c r="R10" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S10" s="100" t="s">
-        <v>167</v>
-      </c>
+      <c r="S10" s="70"/>
       <c r="T10" s="50"/>
       <c r="U10" s="50"/>
       <c r="V10" s="3" t="s">
@@ -2967,9 +2488,7 @@
       <c r="R11" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S11" s="101" t="s">
-        <v>167</v>
-      </c>
+      <c r="S11" s="71"/>
       <c r="T11" s="51"/>
       <c r="U11" s="51"/>
       <c r="V11" s="3" t="s">
@@ -3015,9 +2534,7 @@
       <c r="R12" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S12" s="102" t="s">
-        <v>167</v>
-      </c>
+      <c r="S12" s="72"/>
       <c r="T12" s="52"/>
       <c r="U12" s="52"/>
       <c r="V12" s="3" t="s">
@@ -3030,8 +2547,8 @@
       <c r="A13" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B13" s="81" t="s">
-        <v>163</v>
+      <c r="B13" s="75" t="s">
+        <v>159</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>19</v>
@@ -3079,10 +2596,10 @@
       <c r="R13" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S13" s="80" t="s">
-        <v>164</v>
-      </c>
-      <c r="T13" s="82" t="s">
+      <c r="S13" s="74" t="s">
+        <v>160</v>
+      </c>
+      <c r="T13" s="76" t="s">
         <v>152</v>
       </c>
       <c r="U13" s="57" t="s">
@@ -3102,8 +2619,8 @@
       <c r="A14" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B14" s="60" t="s">
-        <v>153</v>
+      <c r="B14" s="79" t="s">
+        <v>159</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>19</v>
@@ -3151,8 +2668,10 @@
       <c r="R14" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S14" s="59"/>
-      <c r="T14" s="61" t="s">
+      <c r="S14" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="T14" s="80" t="s">
         <v>152</v>
       </c>
       <c r="U14" s="53" t="s">
@@ -3168,7 +2687,7 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
+      <c r="B15" s="77"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="2"/>
@@ -3176,11 +2695,11 @@
       <c r="G15" s="2"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="2" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>140</v>
@@ -3201,11 +2720,15 @@
         <v>149</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="S15" s="54"/>
-      <c r="T15" s="54"/>
-      <c r="U15" s="54"/>
+        <v>130</v>
+      </c>
+      <c r="S15" s="59"/>
+      <c r="T15" s="60" t="s">
+        <v>152</v>
+      </c>
+      <c r="U15" s="53" t="s">
+        <v>151</v>
+      </c>
       <c r="V15" s="3" t="s">
         <v>64</v>
       </c>
@@ -3213,36 +2736,20 @@
       <c r="X15" s="2"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B16" s="84" t="s">
-        <v>166</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="3"/>
       <c r="I16" s="3" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="2" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>140</v>
@@ -3263,46 +2770,56 @@
         <v>149</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="S16" s="83" t="s">
-        <v>165</v>
-      </c>
-      <c r="T16" s="85" t="s">
-        <v>152</v>
-      </c>
-      <c r="U16" s="55" t="s">
-        <v>151</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="S16" s="54"/>
+      <c r="T16" s="54"/>
+      <c r="U16" s="54"/>
       <c r="V16" s="3" t="s">
-        <v>134</v>
+        <v>64</v>
       </c>
       <c r="W16" s="3"/>
-      <c r="X16" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="X16" s="2"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="A17" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" s="82" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>128</v>
+      </c>
       <c r="J17" s="3"/>
-      <c r="K17" s="40" t="s">
+      <c r="K17" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="L17" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="M17" s="67" t="s">
+      <c r="L17" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="N17" s="67" t="s">
+      <c r="M17" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="N17" s="2" t="s">
         <v>140</v>
       </c>
       <c r="O17" s="3" t="s">
@@ -3311,90 +2828,144 @@
       <c r="P17" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="66"/>
-      <c r="T17" s="66"/>
-      <c r="U17" s="66"/>
+      <c r="Q17" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="S17" s="81" t="s">
+        <v>162</v>
+      </c>
+      <c r="T17" s="83" t="s">
+        <v>152</v>
+      </c>
+      <c r="U17" s="55" t="s">
+        <v>151</v>
+      </c>
       <c r="V17" s="3" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="W17" s="3"/>
-      <c r="X17" s="2"/>
+      <c r="X17" s="2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B18" s="63" t="s">
-        <v>153</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="A18" s="3"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-      <c r="K18" s="2" t="s">
+      <c r="K18" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="M18" s="2" t="s">
+      <c r="L18" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="M18" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="N18" s="63" t="s">
         <v>140</v>
       </c>
       <c r="O18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="P18" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="62"/>
+      <c r="T18" s="62"/>
+      <c r="U18" s="62"/>
+      <c r="V18" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="2" t="s">
+      <c r="W18" s="3"/>
+      <c r="X18" s="2"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" s="85" t="s">
+        <v>159</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S18" s="62"/>
-      <c r="T18" s="64" t="s">
-        <v>156</v>
-      </c>
-      <c r="U18" s="55" t="s">
+      <c r="S19" s="84" t="s">
+        <v>163</v>
+      </c>
+      <c r="T19" s="86" t="s">
+        <v>164</v>
+      </c>
+      <c r="U19" s="55" t="s">
         <v>151</v>
       </c>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="2" t="s">
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="2" t="s">
         <v>131</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AB14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="AC7" sqref="AC7"/>
@@ -3402,30 +2973,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -3862,7 +3433,7 @@
       <c r="Y6" s="20"/>
       <c r="Z6" s="15"/>
     </row>
-    <row customFormat="1" r="7" s="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>22</v>
       </c>
@@ -4430,6 +4001,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Addition of Manage Billing Method
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/FCFile.xlsx
+++ b/binaries/FCfiles/FCFile.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SONY\git\qualitesoft\binaries\FCfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{D4EE8EFF-0047-4117-844C-280533D4FD20}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7BCCD6-729B-4573-A6CA-2BE1F3EA437F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="2" tabRatio="449" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="449" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CreateAccount" r:id="rId1" sheetId="5"/>
-    <sheet name="ShipmentInformation" r:id="rId2" sheetId="6"/>
-    <sheet name="Input" r:id="rId3" sheetId="1"/>
-    <sheet name="Marrkups" r:id="rId4" sheetId="4"/>
+    <sheet name="CreateAccount" sheetId="5" r:id="rId1"/>
+    <sheet name="ShipmentInformation" sheetId="6" r:id="rId2"/>
+    <sheet name="Input" sheetId="1" r:id="rId3"/>
+    <sheet name="Marrkups" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="166">
   <si>
     <t>shipmentType</t>
   </si>
@@ -489,18 +489,12 @@
     <t>$1,044.52</t>
   </si>
   <si>
-    <t>07-18-2021</t>
-  </si>
-  <si>
     <t>NPSKU</t>
   </si>
   <si>
     <t>PSKU</t>
   </si>
   <si>
-    <t>$1,055.50</t>
-  </si>
-  <si>
     <t>400</t>
   </si>
   <si>
@@ -513,62 +507,31 @@
     <t>600</t>
   </si>
   <si>
-    <t>07-27-2021</t>
-  </si>
-  <si>
-    <t>51489386</t>
-  </si>
-  <si>
-    <t>08-07-2021</t>
-  </si>
-  <si>
-    <t>51489387</t>
-  </si>
-  <si>
-    <t>51490045</t>
-  </si>
-  <si>
-    <t>08-16-2021</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>51490054</t>
-  </si>
-  <si>
-    <t>51490057</t>
-  </si>
-  <si>
-    <t>51490061</t>
-  </si>
-  <si>
-    <t>51490066</t>
-  </si>
-  <si>
-    <t>51490078</t>
-  </si>
-  <si>
-    <t>51490081</t>
-  </si>
-  <si>
-    <t>51490257</t>
-  </si>
-  <si>
-    <t>51490259</t>
-  </si>
-  <si>
-    <t>51490872</t>
-  </si>
-  <si>
-    <t>51490874</t>
+    <t>08-23-2021</t>
+  </si>
+  <si>
+    <t>51490953</t>
+  </si>
+  <si>
+    <t>51490956</t>
+  </si>
+  <si>
+    <t>51490965</t>
+  </si>
+  <si>
+    <t>51490966</t>
+  </si>
+  <si>
+    <t>$727.51</t>
+  </si>
+  <si>
+    <t>51491260</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -585,7 +548,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="105">
+  <fills count="47">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -760,347 +723,57 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
@@ -1110,7 +783,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="96">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1398,378 +1071,241 @@
       <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="112">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="4" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="3" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="4" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="4" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="5" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="6" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="7" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="7" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="7" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="8" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="9" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="10" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="2" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="6" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="5" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="8" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="13" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="14" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="15" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="16" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="17" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="19" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="18" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="11" fillId="20" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="19" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="12" fillId="21" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="13" fillId="22" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="14" fillId="23" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="15" fillId="24" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="16" fillId="25" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="17" fillId="26" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="17" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="17" fillId="20" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyNumberFormat="1" borderId="0" fillId="4" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="18" fillId="27" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="19" fillId="28" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="20" fillId="29" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="10" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="21" fillId="30" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="22" fillId="31" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="23" fillId="32" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="24" fillId="33" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="25" fillId="34" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="27" fillId="36" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="29" fillId="38" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="31" fillId="40" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="33" fillId="42" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="35" fillId="44" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="37" fillId="46" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="39" fillId="48" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="41" fillId="50" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="43" fillId="52" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="45" fillId="54" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="47" fillId="56" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="49" fillId="58" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="51" fillId="60" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="53" fillId="62" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="55" fillId="64" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="57" fillId="66" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="59" fillId="68" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="61" fillId="70" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="63" fillId="72" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="65" fillId="74" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="67" fillId="76" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="69" fillId="78" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="71" fillId="80" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="73" fillId="82" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="75" fillId="84" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="77" fillId="86" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="79" fillId="88" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="81" fillId="90" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="83" fillId="92" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="85" fillId="94" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="87" fillId="96" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="89" fillId="98" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="91" fillId="100" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="93" fillId="102" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="104" borderId="95" xfId="0" applyFill="true" applyBorder="true"/>
+  <cellXfs count="88">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1786,10 +1322,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1953,21 +1489,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1984,7 +1520,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -2036,15 +1572,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -2052,15 +1588,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="40" width="14.140625" collapsed="true"/>
-    <col min="9" max="9" style="40" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.140625" style="40" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="40" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2122,13 +1658,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -2137,12 +1673,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -2271,43 +1807,42 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="I2" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Y18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:X19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S18"/>
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="17.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="11.43359375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="31.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="17.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="11.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="9" max="10" customWidth="true" style="1" width="33.42578125" collapsed="true"/>
-    <col min="11" max="13" style="1" width="9.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="11.85546875" collapsed="true"/>
-    <col min="15" max="15" style="1" width="9.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="17" max="18" style="1" width="9.140625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="9.95703125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="9.9453125" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="19.28515625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="25" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="17.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="31.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="33.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="13" width="9.140625" style="1" collapsed="1"/>
+    <col min="14" max="14" width="11.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="9.140625" style="1" collapsed="1"/>
+    <col min="16" max="16" width="14.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="18" width="9.140625" style="1" collapsed="1"/>
+    <col min="19" max="20" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="10" style="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="19.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
@@ -2384,7 +1919,7 @@
         <v>129</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -2421,9 +1956,7 @@
       <c r="R2" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S2" s="103" t="s">
-        <v>167</v>
-      </c>
+      <c r="S2" s="73"/>
       <c r="T2" s="42"/>
       <c r="U2" s="42"/>
       <c r="V2" s="3" t="s">
@@ -2481,9 +2014,7 @@
       <c r="R3" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S3" s="89" t="s">
-        <v>169</v>
-      </c>
+      <c r="S3" s="64"/>
       <c r="T3" s="43"/>
       <c r="U3" s="43"/>
       <c r="V3" s="3" t="s">
@@ -2492,7 +2023,7 @@
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
     </row>
-    <row customHeight="1" ht="15.75" r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -2535,7 +2066,7 @@
         <v>18</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>130</v>
@@ -2543,8 +2074,8 @@
       <c r="R4" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S4" s="111" t="s">
-        <v>177</v>
+      <c r="S4" s="87" t="s">
+        <v>165</v>
       </c>
       <c r="T4" s="44"/>
       <c r="U4" s="44" t="s">
@@ -2554,7 +2085,9 @@
         <v>126</v>
       </c>
       <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
+      <c r="X4" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -2609,9 +2142,7 @@
       <c r="R5" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S5" s="93" t="s">
-        <v>171</v>
-      </c>
+      <c r="S5" s="65"/>
       <c r="T5" s="45"/>
       <c r="U5" s="45"/>
       <c r="V5" s="3" t="s">
@@ -2671,9 +2202,7 @@
       <c r="R6" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S6" s="94" t="s">
-        <v>167</v>
-      </c>
+      <c r="S6" s="66"/>
       <c r="T6" s="46"/>
       <c r="U6" s="46"/>
       <c r="V6" s="3" t="s">
@@ -2719,9 +2248,7 @@
       <c r="R7" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S7" s="95" t="s">
-        <v>167</v>
-      </c>
+      <c r="S7" s="67"/>
       <c r="T7" s="47"/>
       <c r="U7" s="47"/>
       <c r="V7" s="3" t="s">
@@ -2781,9 +2308,7 @@
       <c r="R8" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S8" s="97" t="s">
-        <v>172</v>
-      </c>
+      <c r="S8" s="68"/>
       <c r="T8" s="48"/>
       <c r="U8" s="48"/>
       <c r="V8" s="3" t="s">
@@ -2843,9 +2368,7 @@
       <c r="R9" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S9" s="99" t="s">
-        <v>173</v>
-      </c>
+      <c r="S9" s="69"/>
       <c r="T9" s="49"/>
       <c r="U9" s="49"/>
       <c r="V9" s="3" t="s">
@@ -2905,9 +2428,7 @@
       <c r="R10" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S10" s="100" t="s">
-        <v>167</v>
-      </c>
+      <c r="S10" s="70"/>
       <c r="T10" s="50"/>
       <c r="U10" s="50"/>
       <c r="V10" s="3" t="s">
@@ -2967,9 +2488,7 @@
       <c r="R11" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S11" s="101" t="s">
-        <v>167</v>
-      </c>
+      <c r="S11" s="71"/>
       <c r="T11" s="51"/>
       <c r="U11" s="51"/>
       <c r="V11" s="3" t="s">
@@ -3015,9 +2534,7 @@
       <c r="R12" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S12" s="102" t="s">
-        <v>167</v>
-      </c>
+      <c r="S12" s="72"/>
       <c r="T12" s="52"/>
       <c r="U12" s="52"/>
       <c r="V12" s="3" t="s">
@@ -3030,8 +2547,8 @@
       <c r="A13" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B13" s="81" t="s">
-        <v>163</v>
+      <c r="B13" s="75" t="s">
+        <v>159</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>19</v>
@@ -3079,10 +2596,10 @@
       <c r="R13" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S13" s="80" t="s">
-        <v>164</v>
-      </c>
-      <c r="T13" s="82" t="s">
+      <c r="S13" s="74" t="s">
+        <v>160</v>
+      </c>
+      <c r="T13" s="76" t="s">
         <v>152</v>
       </c>
       <c r="U13" s="57" t="s">
@@ -3102,8 +2619,8 @@
       <c r="A14" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B14" s="60" t="s">
-        <v>153</v>
+      <c r="B14" s="79" t="s">
+        <v>159</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>19</v>
@@ -3151,8 +2668,10 @@
       <c r="R14" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S14" s="59"/>
-      <c r="T14" s="61" t="s">
+      <c r="S14" s="78" t="s">
+        <v>161</v>
+      </c>
+      <c r="T14" s="80" t="s">
         <v>152</v>
       </c>
       <c r="U14" s="53" t="s">
@@ -3168,7 +2687,7 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
+      <c r="B15" s="77"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="2"/>
@@ -3176,11 +2695,11 @@
       <c r="G15" s="2"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="2" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>140</v>
@@ -3201,11 +2720,15 @@
         <v>149</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="S15" s="54"/>
-      <c r="T15" s="54"/>
-      <c r="U15" s="54"/>
+        <v>130</v>
+      </c>
+      <c r="S15" s="59"/>
+      <c r="T15" s="60" t="s">
+        <v>152</v>
+      </c>
+      <c r="U15" s="53" t="s">
+        <v>151</v>
+      </c>
       <c r="V15" s="3" t="s">
         <v>64</v>
       </c>
@@ -3213,36 +2736,20 @@
       <c r="X15" s="2"/>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B16" s="84" t="s">
-        <v>166</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="3"/>
       <c r="I16" s="3" t="s">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="2" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>140</v>
@@ -3263,46 +2770,56 @@
         <v>149</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="S16" s="83" t="s">
-        <v>165</v>
-      </c>
-      <c r="T16" s="85" t="s">
-        <v>152</v>
-      </c>
-      <c r="U16" s="55" t="s">
-        <v>151</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="S16" s="54"/>
+      <c r="T16" s="54"/>
+      <c r="U16" s="54"/>
       <c r="V16" s="3" t="s">
-        <v>134</v>
+        <v>64</v>
       </c>
       <c r="W16" s="3"/>
-      <c r="X16" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="X16" s="2"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="A17" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" s="82" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>128</v>
+      </c>
       <c r="J17" s="3"/>
-      <c r="K17" s="40" t="s">
+      <c r="K17" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="L17" s="40" t="s">
-        <v>158</v>
-      </c>
-      <c r="M17" s="67" t="s">
+      <c r="L17" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="N17" s="67" t="s">
+      <c r="M17" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="N17" s="2" t="s">
         <v>140</v>
       </c>
       <c r="O17" s="3" t="s">
@@ -3311,90 +2828,144 @@
       <c r="P17" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="66"/>
-      <c r="T17" s="66"/>
-      <c r="U17" s="66"/>
+      <c r="Q17" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="S17" s="81" t="s">
+        <v>162</v>
+      </c>
+      <c r="T17" s="83" t="s">
+        <v>152</v>
+      </c>
+      <c r="U17" s="55" t="s">
+        <v>151</v>
+      </c>
       <c r="V17" s="3" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="W17" s="3"/>
-      <c r="X17" s="2"/>
+      <c r="X17" s="2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B18" s="63" t="s">
-        <v>153</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="A18" s="3"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
       <c r="J18" s="3"/>
-      <c r="K18" s="2" t="s">
+      <c r="K18" s="40" t="s">
         <v>141</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="M18" s="2" t="s">
+      <c r="L18" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="M18" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="N18" s="2" t="s">
+      <c r="N18" s="63" t="s">
         <v>140</v>
       </c>
       <c r="O18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="P18" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="62"/>
+      <c r="T18" s="62"/>
+      <c r="U18" s="62"/>
+      <c r="V18" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="Q18" s="3"/>
-      <c r="R18" s="2" t="s">
+      <c r="W18" s="3"/>
+      <c r="X18" s="2"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" s="85" t="s">
+        <v>159</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="S18" s="62"/>
-      <c r="T18" s="64" t="s">
-        <v>156</v>
-      </c>
-      <c r="U18" s="55" t="s">
+      <c r="S19" s="84" t="s">
+        <v>163</v>
+      </c>
+      <c r="T19" s="86" t="s">
+        <v>164</v>
+      </c>
+      <c r="U19" s="55" t="s">
         <v>151</v>
       </c>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="2" t="s">
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="2" t="s">
         <v>131</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AB14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="AC7" sqref="AC7"/>
@@ -3402,30 +2973,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -3862,7 +3433,7 @@
       <c r="Y6" s="20"/>
       <c r="Z6" s="15"/>
     </row>
-    <row customFormat="1" r="7" s="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>22</v>
       </c>
@@ -4430,6 +4001,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>